<commit_message>
Change Colorado Counties geojson to WGS 84 and update xlsx file and README to reflect changes
</commit_message>
<xml_diff>
--- a/data/Colorado-Counties.xlsx
+++ b/data/Colorado-Counties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -713,32 +713,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Colorado's rivers are categorized into 9 major river basins as part of the Interbasin Compact Committee (IBCC).  A GIS shapefile of the basins can be found within the Colorado Water Conservation Board (CWCB)'s Data Viewer:  https://www.coloradodnr.info/h5v/Index.html?viewer=cwcbviewer.  The IBCC Basin layer is within the Admin Boundary category.  OWF saved the shapefile in GeoJSON format, which can be found at:  data-orig/Colorado-IBCC-Basins.geojson.  Several counties are in more than one IBCC basin.  In these cases, each basin is listed and values are separated by commas.  Counties in multiple basins can also be found in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>County_Basin_Relate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> worksheet.  </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Geographic Names Information System (</t>
     </r>
     <r>
@@ -876,21 +850,6 @@
     <t>CO</t>
   </si>
   <si>
-    <r>
-      <t>A GIS shapefile of the counties can be found within the Colorado Water Conservation Board (CWCB)'s Data Viewer:  https://www.coloradodnr.info/h5v/Index.html?viewer=cwcbviewer.  The County layer is within the Admin Boundary category.  OWF saved the shapefile in GeoJSON format, which can be found at:  data-orig/Colorado-Counties.geojson.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-  </si>
-  <si>
     <t>Basin_Fraction</t>
   </si>
   <si>
@@ -1461,6 +1420,35 @@
   </si>
   <si>
     <t>63012</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Colorado's rivers are categorized into 9 major river basins as part of the Interbasin Compact Committee (IBCC).  A GIS shapefile of the basins can be found within the Colorado Water Conservation Board (CWCB)'s Data Viewer:  https://www.coloradodnr.info/h5v/Index.html?viewer=cwcbviewer.  The IBCC Basin layer is within the Admin Boundary category.  OWF saved the shapefile in GeoJSON format and converted the coordinate reference system to WGS 84, which can be found at:  data-orig/Colorado-IBCC-Basins-WGS84.geojson.  Several counties are in more than one IBCC basin.  In these cases, each basin is listed and values are separated by commas.  Counties in multiple basins can also be found in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>County_Basin_Relate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> worksheet.  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A GIS shapefile of the counties can be found within the Colorado Water Conservation Board (CWCB)'s Data Viewer:  https://www.coloradodnr.info/h5v/Index.html?viewer=cwcbviewer.  The County layer is within the Admin Boundary category.  OWF saved the shapefile in GeoJSON format and converted the coordinate reference system to WGS 84, which can be found at:  data-orig/Colorado-Counties-WGS84.geojson.  </t>
   </si>
 </sst>
 </file>
@@ -1655,33 +1643,88 @@
   <dxfs count="18">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1735,6 +1778,91 @@
           <color theme="4" tint="0.39997558519241921"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1844,176 +1972,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -2071,6 +2029,36 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2497,21 +2485,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L65" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L65" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A1:L65"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="CountyName" dataDxfId="14"/>
-    <tableColumn id="2" name="State_Abbrev" dataDxfId="7"/>
-    <tableColumn id="14" name="FIPS_ID" dataDxfId="5"/>
-    <tableColumn id="4" name="FIPS_ID_Flag" dataDxfId="6"/>
-    <tableColumn id="5" name="FIPS_wState_ID" dataDxfId="13"/>
-    <tableColumn id="6" name="GNIS_ID" dataDxfId="12"/>
-    <tableColumn id="7" name="GNIS_ID_Flag" dataDxfId="11"/>
-    <tableColumn id="15" name="DOLA_LG_ID" dataDxfId="3"/>
-    <tableColumn id="9" name="DOLA_LG_ID_Flag" dataDxfId="4"/>
-    <tableColumn id="10" name="IBCC_Basin_CSV" dataDxfId="10"/>
-    <tableColumn id="11" name="Num_IBCC_Basin" dataDxfId="9"/>
-    <tableColumn id="12" name="Comment" dataDxfId="8"/>
+    <tableColumn id="1" name="CountyName" dataDxfId="11"/>
+    <tableColumn id="2" name="State_Abbrev" dataDxfId="10"/>
+    <tableColumn id="14" name="FIPS_ID" dataDxfId="9"/>
+    <tableColumn id="4" name="FIPS_ID_Flag" dataDxfId="8"/>
+    <tableColumn id="5" name="FIPS_wState_ID" dataDxfId="7"/>
+    <tableColumn id="6" name="GNIS_ID" dataDxfId="6"/>
+    <tableColumn id="7" name="GNIS_ID_Flag" dataDxfId="5"/>
+    <tableColumn id="15" name="DOLA_LG_ID" dataDxfId="4"/>
+    <tableColumn id="9" name="DOLA_LG_ID_Flag" dataDxfId="3"/>
+    <tableColumn id="10" name="IBCC_Basin_CSV" dataDxfId="2"/>
+    <tableColumn id="11" name="Num_IBCC_Basin" dataDxfId="1"/>
+    <tableColumn id="12" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2782,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2787,7 @@
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2839,7 +2827,7 @@
     </row>
     <row r="4" spans="1:17" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2879,7 +2867,7 @@
     </row>
     <row r="6" spans="1:17" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2919,7 +2907,7 @@
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>133</v>
+        <v>332</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2957,9 +2945,9 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>150</v>
+        <v>333</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2999,17 +2987,17 @@
     </row>
     <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3029,12 +3017,12 @@
     </row>
     <row r="21" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3046,7 +3034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1:Q1048576"/>
     </sheetView>
   </sheetViews>
@@ -3068,34 +3056,34 @@
         <v>65</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>117</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F1" s="29" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H1" s="29" t="s">
         <v>118</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L1" s="29" t="s">
         <v>128</v>
@@ -3106,31 +3094,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>66</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F2" s="20">
         <v>198116</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>119</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K2" s="22">
         <v>2</v>
@@ -3142,13 +3130,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>126</v>
@@ -3157,13 +3145,13 @@
         <v>198117</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>120</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>44</v>
@@ -3178,31 +3166,31 @@
         <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="30" t="s">
         <v>68</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F4" s="20">
         <v>198118</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H4" s="30" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K4" s="22">
         <v>2</v>
@@ -3214,31 +3202,31 @@
         <v>7</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F5" s="25">
         <v>198119</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>122</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K5" s="27">
         <v>2</v>
@@ -3250,31 +3238,31 @@
         <v>12</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F6" s="20">
         <v>198120</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K6" s="22">
         <v>1</v>
@@ -3286,31 +3274,31 @@
         <v>16</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>71</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F7" s="25">
         <v>198121</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K7" s="27">
         <v>1</v>
@@ -3322,31 +3310,31 @@
         <v>13</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F8" s="20">
         <v>198122</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H8" s="30" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K8" s="22">
         <v>1</v>
@@ -3358,31 +3346,31 @@
         <v>21</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F9" s="25">
         <v>1945881</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K9" s="27">
         <v>2</v>
@@ -3394,31 +3382,31 @@
         <v>23</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F10" s="20">
         <v>198123</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>126</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K10" s="22">
         <v>1</v>
@@ -3430,31 +3418,31 @@
         <v>32</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F11" s="25">
         <v>198124</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>127</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K11" s="27">
         <v>2</v>
@@ -3466,31 +3454,31 @@
         <v>41</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>76</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="20">
         <v>198125</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K12" s="22">
         <v>1</v>
@@ -3502,31 +3490,31 @@
         <v>5</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F13" s="25">
         <v>198126</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K13" s="27">
         <v>2</v>
@@ -3538,31 +3526,31 @@
         <v>19</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F14" s="20">
         <v>198127</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K14" s="22">
         <v>2</v>
@@ -3574,31 +3562,31 @@
         <v>52</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>79</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F15" s="25">
         <v>198128</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K15" s="27">
         <v>1</v>
@@ -3610,31 +3598,31 @@
         <v>53</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>80</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F16" s="20">
         <v>198129</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K16" s="22">
         <v>1</v>
@@ -3646,28 +3634,28 @@
         <v>27</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F17" s="25">
         <v>198130</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>39</v>
@@ -3682,31 +3670,31 @@
         <v>36</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F18" s="20">
         <v>198131</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K18" s="22">
         <v>2</v>
@@ -3718,31 +3706,31 @@
         <v>54</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>83</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F19" s="25">
         <v>198132</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K19" s="27">
         <v>1</v>
@@ -3754,31 +3742,31 @@
         <v>25</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F20" s="20">
         <v>198133</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K20" s="22">
         <v>1</v>
@@ -3790,31 +3778,31 @@
         <v>14</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F21" s="25">
         <v>198134</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K21" s="27">
         <v>1</v>
@@ -3826,31 +3814,31 @@
         <v>18</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>87</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F22" s="20">
         <v>198135</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K22" s="22">
         <v>2</v>
@@ -3862,31 +3850,31 @@
         <v>1</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>86</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F23" s="25">
         <v>198136</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K23" s="27">
         <v>3</v>
@@ -3898,31 +3886,31 @@
         <v>26</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F24" s="20">
         <v>198137</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K24" s="22">
         <v>1</v>
@@ -3934,31 +3922,31 @@
         <v>38</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F25" s="25">
         <v>198138</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K25" s="27">
         <v>2</v>
@@ -3970,31 +3958,31 @@
         <v>29</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>90</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F26" s="20">
         <v>198139</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K26" s="22">
         <v>1</v>
@@ -4006,31 +3994,31 @@
         <v>57</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>91</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F27" s="25">
         <v>198140</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K27" s="27">
         <v>2</v>
@@ -4042,31 +4030,31 @@
         <v>39</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F28" s="20">
         <v>198141</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K28" s="22">
         <v>2</v>
@@ -4078,31 +4066,31 @@
         <v>58</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>93</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F29" s="25">
         <v>198142</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K29" s="27">
         <v>3</v>
@@ -4114,31 +4102,31 @@
         <v>49</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>94</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F30" s="20">
         <v>198143</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K30" s="22">
         <v>1</v>
@@ -4150,31 +4138,31 @@
         <v>59</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="30" t="s">
         <v>95</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F31" s="25">
         <v>198144</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K31" s="27">
         <v>1</v>
@@ -4186,31 +4174,31 @@
         <v>30</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>96</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F32" s="20">
         <v>198145</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K32" s="22">
         <v>2</v>
@@ -4222,31 +4210,31 @@
         <v>55</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>97</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F33" s="25">
         <v>198146</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K33" s="27">
         <v>1</v>
@@ -4258,31 +4246,31 @@
         <v>24</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>98</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F34" s="20">
         <v>198147</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J34" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K34" s="22">
         <v>1</v>
@@ -4294,31 +4282,31 @@
         <v>15</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F35" s="25">
         <v>198148</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J35" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K35" s="27">
         <v>1</v>
@@ -4330,31 +4318,31 @@
         <v>43</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>99</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F36" s="20">
         <v>198149</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K36" s="22">
         <v>1</v>
@@ -4366,31 +4354,31 @@
         <v>17</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C37" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F37" s="25">
         <v>198150</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K37" s="27">
         <v>2</v>
@@ -4402,31 +4390,31 @@
         <v>2</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>102</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F38" s="20">
         <v>198151</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K38" s="22">
         <v>1</v>
@@ -4438,31 +4426,31 @@
         <v>8</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C39" s="30" t="s">
         <v>103</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F39" s="25">
         <v>198152</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K39" s="27">
         <v>2</v>
@@ -4474,31 +4462,31 @@
         <v>48</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" s="30" t="s">
         <v>104</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F40" s="20">
         <v>198153</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K40" s="22">
         <v>1</v>
@@ -4510,31 +4498,31 @@
         <v>37</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>105</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F41" s="25">
         <v>198154</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J41" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K41" s="27">
         <v>3</v>
@@ -4546,31 +4534,31 @@
         <v>51</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="30" t="s">
         <v>106</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F42" s="20">
         <v>198155</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K42" s="22">
         <v>2</v>
@@ -4582,31 +4570,31 @@
         <v>34</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F43" s="25">
         <v>198156</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J43" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K43" s="27">
         <v>1</v>
@@ -4618,31 +4606,31 @@
         <v>33</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" s="30" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F44" s="20">
         <v>198157</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K44" s="22">
         <v>1</v>
@@ -4654,31 +4642,31 @@
         <v>45</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C45" s="30" t="s">
         <v>109</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F45" s="25">
         <v>198158</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J45" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K45" s="27">
         <v>2</v>
@@ -4690,31 +4678,31 @@
         <v>22</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" s="30" t="s">
         <v>110</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F46" s="20">
         <v>198159</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K46" s="22">
         <v>1</v>
@@ -4726,31 +4714,31 @@
         <v>31</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C47" s="30" t="s">
         <v>111</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F47" s="25">
         <v>198160</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K47" s="27">
         <v>1</v>
@@ -4762,28 +4750,28 @@
         <v>46</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C48" s="30" t="s">
         <v>112</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F48" s="20">
         <v>198161</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J48" s="21" t="s">
         <v>39</v>
@@ -4798,31 +4786,31 @@
         <v>56</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C49" s="30" t="s">
         <v>113</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F49" s="25">
         <v>198162</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I49" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J49" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K49" s="27">
         <v>2</v>
@@ -4834,31 +4822,31 @@
         <v>40</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C50" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F50" s="20">
         <v>198163</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K50" s="22">
         <v>1</v>
@@ -4870,31 +4858,31 @@
         <v>9</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C51" s="30" t="s">
         <v>115</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F51" s="25">
         <v>198164</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K51" s="27">
         <v>1</v>
@@ -4906,31 +4894,31 @@
         <v>42</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C52" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F52" s="20">
         <v>198165</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K52" s="22">
         <v>1</v>
@@ -4942,31 +4930,31 @@
         <v>11</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F53" s="25">
         <v>198166</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K53" s="27">
         <v>1</v>
@@ -4978,31 +4966,31 @@
         <v>61</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F54" s="20">
         <v>198167</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J54" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K54" s="22">
         <v>1</v>
@@ -5014,31 +5002,31 @@
         <v>44</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F55" s="25">
         <v>198168</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J55" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K55" s="27">
         <v>2</v>
@@ -5050,31 +5038,31 @@
         <v>47</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F56" s="20">
         <v>198169</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K56" s="22">
         <v>2</v>
@@ -5086,31 +5074,31 @@
         <v>28</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F57" s="25">
         <v>198170</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J57" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K57" s="27">
         <v>3</v>
@@ -5122,31 +5110,31 @@
         <v>63</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F58" s="20">
         <v>198171</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J58" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K58" s="22">
         <v>3</v>
@@ -5158,31 +5146,31 @@
         <v>62</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F59" s="25">
         <v>198172</v>
       </c>
       <c r="G59" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J59" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K59" s="27">
         <v>1</v>
@@ -5194,31 +5182,31 @@
         <v>60</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F60" s="20">
         <v>198173</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K60" s="22">
         <v>1</v>
@@ -5230,31 +5218,31 @@
         <v>20</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F61" s="25">
         <v>198174</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H61" s="30" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J61" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K61" s="27">
         <v>1</v>
@@ -5266,31 +5254,31 @@
         <v>35</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F62" s="20">
         <v>198175</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K62" s="22">
         <v>2</v>
@@ -5302,31 +5290,31 @@
         <v>3</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E63" s="24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F63" s="25">
         <v>198176</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J63" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K63" s="27">
         <v>1</v>
@@ -5338,31 +5326,31 @@
         <v>10</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F64" s="20">
         <v>198177</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I64" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J64" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K64" s="22">
         <v>1</v>
@@ -5374,31 +5362,31 @@
         <v>50</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F65" s="25">
         <v>198178</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H65" s="30" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J65" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K65" s="27">
         <v>1</v>
@@ -5407,13 +5395,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:L1">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="County">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="County">
       <formula>NOT(ISERROR(SEARCH("County",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Town of">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Town of">
       <formula>NOT(ISERROR(SEARCH("Town of",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="City of">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="City of">
       <formula>NOT(ISERROR(SEARCH("City of",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5449,10 +5437,10 @@
         <v>65</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5464,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2">
         <v>0.24</v>
@@ -5479,7 +5467,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3">
         <v>0.76</v>
@@ -5494,7 +5482,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4">
         <v>0.28999999999999998</v>
@@ -5509,7 +5497,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5">
         <v>0.71</v>
@@ -5539,7 +5527,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7">
         <v>0.95</v>
@@ -5554,7 +5542,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8">
         <v>0.46</v>
@@ -5569,7 +5557,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9">
         <v>0.54</v>
@@ -5584,7 +5572,7 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D10">
         <v>0.39</v>
@@ -5599,7 +5587,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D11">
         <v>0.61</v>
@@ -5614,7 +5602,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12">
         <v>0.01</v>
@@ -5644,7 +5632,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14">
         <v>0.03</v>
@@ -5674,7 +5662,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D16">
         <v>0.11</v>
@@ -5689,7 +5677,7 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17">
         <v>0.89</v>
@@ -5704,7 +5692,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18">
         <v>0.02</v>
@@ -5719,7 +5707,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19">
         <v>0.03</v>
@@ -5734,7 +5722,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20">
         <v>0.95</v>
@@ -5749,7 +5737,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D21">
         <v>0.02</v>
@@ -5764,7 +5752,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22">
         <v>0.32</v>
@@ -5779,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23">
         <v>0.66</v>
@@ -5794,7 +5782,7 @@
         <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D24">
         <v>0.15</v>
@@ -5809,7 +5797,7 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D25">
         <v>0.85</v>
@@ -5824,7 +5812,7 @@
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D26">
         <v>0.01</v>
@@ -5839,7 +5827,7 @@
         <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27">
         <v>0.99</v>
@@ -5854,7 +5842,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28">
         <v>0.03</v>
@@ -5884,7 +5872,7 @@
         <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D30">
         <v>0.26</v>
@@ -5929,7 +5917,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D33">
         <v>0.38</v>
@@ -5944,7 +5932,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D34">
         <v>0.62</v>
@@ -5959,7 +5947,7 @@
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35">
         <v>0.16</v>
@@ -5974,7 +5962,7 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D36">
         <v>0.84</v>
@@ -5989,7 +5977,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37">
         <v>0.27</v>
@@ -6004,7 +5992,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38">
         <v>0.73</v>
@@ -6019,7 +6007,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D39">
         <v>0.23</v>
@@ -6049,7 +6037,7 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D41">
         <v>0.54</v>
@@ -6064,7 +6052,7 @@
         <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D42">
         <v>0.25</v>
@@ -6094,7 +6082,7 @@
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D44">
         <v>0.5</v>
@@ -6124,7 +6112,7 @@
         <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D46">
         <v>0.13</v>
@@ -6139,7 +6127,7 @@
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D47">
         <v>0.87</v>
@@ -6154,7 +6142,7 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D48">
         <v>0.01</v>
@@ -6184,7 +6172,7 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D50">
         <v>0.11</v>
@@ -6199,7 +6187,7 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51">
         <v>0.89</v>
@@ -6214,7 +6202,7 @@
         <v>28</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52">
         <v>0.01</v>
@@ -6289,7 +6277,7 @@
         <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D57">
         <v>0.89</v>
@@ -6304,7 +6292,7 @@
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58">
         <v>0.15</v>
@@ -6319,7 +6307,7 @@
         <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59">
         <v>0.28999999999999998</v>
@@ -6334,7 +6322,7 @@
         <v>35</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D60">
         <v>0.56000000000000005</v>
@@ -6369,27 +6357,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -6399,12 +6387,12 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -6414,17 +6402,17 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -6449,13 +6437,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6463,10 +6451,10 @@
         <v>43046</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6528,19 +6516,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6548,33 +6536,33 @@
         <v>65</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6582,50 +6570,50 @@
         <v>117</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6633,33 +6621,33 @@
         <v>64</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6667,67 +6655,67 @@
         <v>118</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6735,16 +6723,16 @@
         <v>128</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>180</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add TOC to README
</commit_message>
<xml_diff>
--- a/data/Colorado-Counties.xlsx
+++ b/data/Colorado-Counties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -1231,32 +1231,6 @@
     <t>125</t>
   </si>
   <si>
-    <r>
-      <t>Federal Information Processing Standard (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FIPS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) codes are available from the U.S. Census Bureau:  https://www.census.gov/geo/reference/codes/cou.html.  Data were downloaded on 2017-11-07.  Data are available as text files.  OWF saved the data as a comma-separated text file, which can be found at:  data-orig/Colorado-FIPS-Counties.txt.</t>
-    </r>
-  </si>
-  <si>
     <t>64030</t>
   </si>
   <si>
@@ -1449,6 +1423,32 @@
   </si>
   <si>
     <t xml:space="preserve">A GIS shapefile of the counties can be found within the Colorado Water Conservation Board (CWCB)'s Data Viewer:  https://www.coloradodnr.info/h5v/Index.html?viewer=cwcbviewer.  The County layer is within the Admin Boundary category.  OWF saved the shapefile in GeoJSON format and converted the coordinate reference system to WGS 84, which can be found at:  data-orig/Colorado-Counties-WGS84.geojson.  </t>
+  </si>
+  <si>
+    <r>
+      <t>Federal Information Processing Standard (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FIPS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) codes are available from the U.S. Census Bureau:  https://www.census.gov/geo/reference/codes/cou.html.  Data were downloaded on 2017-11-07.  Data are available as text files.  OWF saved the data as a comma-separated text file, which can be found at:  data-orig/Colorado-FIPS-Counties.csv.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2770,7 +2770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>276</v>
+        <v>333</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="8" spans="1:17" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="10" spans="1:17" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3034,8 +3034,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:Q1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3364,7 +3367,7 @@
         <v>167</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I9" s="24" t="s">
         <v>167</v>
@@ -3472,7 +3475,7 @@
         <v>167</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>167</v>
@@ -3508,7 +3511,7 @@
         <v>167</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I13" s="24" t="s">
         <v>167</v>
@@ -3544,7 +3547,7 @@
         <v>167</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>167</v>
@@ -3580,7 +3583,7 @@
         <v>167</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>167</v>
@@ -3616,7 +3619,7 @@
         <v>167</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>167</v>
@@ -3652,7 +3655,7 @@
         <v>167</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>167</v>
@@ -3688,7 +3691,7 @@
         <v>167</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>167</v>
@@ -3724,7 +3727,7 @@
         <v>167</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>167</v>
@@ -3760,7 +3763,7 @@
         <v>167</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I20" s="19" t="s">
         <v>167</v>
@@ -3796,7 +3799,7 @@
         <v>167</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>167</v>
@@ -3832,7 +3835,7 @@
         <v>167</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I22" s="19" t="s">
         <v>167</v>
@@ -3868,7 +3871,7 @@
         <v>167</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>167</v>
@@ -3904,7 +3907,7 @@
         <v>167</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>167</v>
@@ -3940,7 +3943,7 @@
         <v>167</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I25" s="24" t="s">
         <v>167</v>
@@ -3976,7 +3979,7 @@
         <v>167</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>167</v>
@@ -4012,7 +4015,7 @@
         <v>167</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I27" s="24" t="s">
         <v>167</v>
@@ -4048,7 +4051,7 @@
         <v>167</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>167</v>
@@ -4084,7 +4087,7 @@
         <v>167</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I29" s="24" t="s">
         <v>167</v>
@@ -4120,7 +4123,7 @@
         <v>167</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I30" s="19" t="s">
         <v>167</v>
@@ -4156,7 +4159,7 @@
         <v>167</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>167</v>
@@ -4192,7 +4195,7 @@
         <v>167</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>167</v>
@@ -4228,7 +4231,7 @@
         <v>167</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I33" s="24" t="s">
         <v>167</v>
@@ -4264,7 +4267,7 @@
         <v>167</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I34" s="19" t="s">
         <v>167</v>
@@ -4300,7 +4303,7 @@
         <v>167</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I35" s="24" t="s">
         <v>167</v>
@@ -4336,7 +4339,7 @@
         <v>167</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>167</v>
@@ -4372,7 +4375,7 @@
         <v>167</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I37" s="24" t="s">
         <v>167</v>
@@ -4408,7 +4411,7 @@
         <v>167</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I38" s="19" t="s">
         <v>167</v>
@@ -4444,7 +4447,7 @@
         <v>167</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I39" s="24" t="s">
         <v>167</v>
@@ -4480,7 +4483,7 @@
         <v>167</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>167</v>
@@ -4516,7 +4519,7 @@
         <v>167</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I41" s="24" t="s">
         <v>167</v>
@@ -4552,7 +4555,7 @@
         <v>167</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I42" s="19" t="s">
         <v>167</v>
@@ -4588,7 +4591,7 @@
         <v>167</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I43" s="24" t="s">
         <v>167</v>
@@ -4624,7 +4627,7 @@
         <v>167</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>167</v>
@@ -4660,7 +4663,7 @@
         <v>167</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I45" s="24" t="s">
         <v>167</v>
@@ -4696,7 +4699,7 @@
         <v>167</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>167</v>
@@ -4732,7 +4735,7 @@
         <v>167</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I47" s="24" t="s">
         <v>167</v>
@@ -4768,7 +4771,7 @@
         <v>167</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I48" s="19" t="s">
         <v>167</v>
@@ -4804,7 +4807,7 @@
         <v>167</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I49" s="24" t="s">
         <v>167</v>
@@ -4840,7 +4843,7 @@
         <v>167</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>167</v>
@@ -4876,7 +4879,7 @@
         <v>167</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I51" s="24" t="s">
         <v>167</v>
@@ -4912,7 +4915,7 @@
         <v>167</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I52" s="19" t="s">
         <v>167</v>
@@ -4948,7 +4951,7 @@
         <v>167</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I53" s="24" t="s">
         <v>167</v>
@@ -4984,7 +4987,7 @@
         <v>167</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>167</v>
@@ -5020,7 +5023,7 @@
         <v>167</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I55" s="24" t="s">
         <v>167</v>
@@ -5056,7 +5059,7 @@
         <v>167</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I56" s="19" t="s">
         <v>167</v>
@@ -5092,7 +5095,7 @@
         <v>167</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I57" s="24" t="s">
         <v>167</v>
@@ -5128,7 +5131,7 @@
         <v>167</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I58" s="19" t="s">
         <v>167</v>
@@ -5164,7 +5167,7 @@
         <v>167</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I59" s="24" t="s">
         <v>167</v>
@@ -5200,7 +5203,7 @@
         <v>167</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I60" s="19" t="s">
         <v>167</v>
@@ -5236,7 +5239,7 @@
         <v>167</v>
       </c>
       <c r="H61" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I61" s="24" t="s">
         <v>167</v>
@@ -5272,7 +5275,7 @@
         <v>167</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>167</v>
@@ -5308,7 +5311,7 @@
         <v>167</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I63" s="24" t="s">
         <v>167</v>
@@ -5344,7 +5347,7 @@
         <v>167</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I64" s="19" t="s">
         <v>167</v>
@@ -5380,7 +5383,7 @@
         <v>167</v>
       </c>
       <c r="H65" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I65" s="24" t="s">
         <v>167</v>

</xml_diff>